<commit_message>
Further work to $VFC
</commit_message>
<xml_diff>
--- a/$VFC.xlsx
+++ b/$VFC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6028FAC-09F3-4D48-A391-D1259DC56672}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BB5435-CB30-4A98-94D0-D8E6EC9C04D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{CCA103E1-675A-4605-B96F-0654FEFE97EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CCA103E1-675A-4605-B96F-0654FEFE97EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -4448,6 +4448,8 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4457,16 +4459,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4487,14 +4495,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4517,16 +4517,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>176522</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>97023</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>271772</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>20823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>271088</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>366338</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4556,7 +4556,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2614922" y="97023"/>
+          <a:off x="2100572" y="182748"/>
           <a:ext cx="1313766" cy="436378"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4983,8 +4983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC19E0CD-5502-4D8A-82C5-8B7A2CE78084}">
   <dimension ref="A2:Z40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5005,45 +5005,37 @@
       <c r="Q3"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="H4" s="49" t="s">
+      <c r="R4" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="53"/>
+      <c r="W4" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="X4" s="52"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="53"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B5" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="G5" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="51"/>
-      <c r="R4" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="51"/>
-      <c r="W4" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="51"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B5" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="51"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="10"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="53"/>
       <c r="R5" s="7" t="s">
         <v>13</v>
       </c>
@@ -5067,12 +5059,9 @@
         <v>27.84</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="H6" s="29">
-        <v>44743</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -5103,19 +5092,20 @@
       <c r="D7" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="30" t="s">
-        <v>91</v>
-      </c>
+      <c r="G7" s="29">
+        <v>44743</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
-      <c r="P7" s="31" t="s">
-        <v>73</v>
-      </c>
+      <c r="P7" s="10"/>
       <c r="R7" s="18" t="s">
         <v>18</v>
       </c>
@@ -5136,7 +5126,10 @@
         <v>10827.02240928</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="H8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="30" t="s">
+        <v>91</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -5144,7 +5137,9 @@
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
-      <c r="P8" s="10"/>
+      <c r="P8" s="31" t="s">
+        <v>73</v>
+      </c>
       <c r="R8" s="18" t="s">
         <v>19</v>
       </c>
@@ -5168,7 +5163,8 @@
       <c r="D9" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -5199,7 +5195,8 @@
       <c r="D10" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -5230,7 +5227,8 @@
       <c r="D11" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -5259,7 +5257,8 @@
         <v>15595.92240928</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="H12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -5278,7 +5277,8 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="H13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -5299,7 +5299,8 @@
       <c r="Z13" s="10"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="H14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
@@ -5320,12 +5321,13 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
-      <c r="H15" s="19"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -5352,11 +5354,12 @@
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="53"/>
-      <c r="H16" s="19"/>
+      <c r="D16" s="59"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -5379,11 +5382,12 @@
       <c r="B17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="H17" s="19"/>
+      <c r="D17" s="59"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -5403,7 +5407,8 @@
       <c r="B18" s="13"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
-      <c r="H18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -5426,11 +5431,12 @@
       <c r="B19" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="63"/>
-      <c r="H19" s="19"/>
+      <c r="D19" s="55"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -5447,7 +5453,8 @@
       <c r="U19" s="10"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="H20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5462,7 +5469,8 @@
       <c r="U20" s="10"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="H21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5479,12 +5487,13 @@
       <c r="U21" s="10"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
-      <c r="H22" s="19"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5504,19 +5513,20 @@
       <c r="B23" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="53"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="12"/>
+      <c r="D23" s="59"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="10"/>
       <c r="R23" s="18" t="s">
         <v>30</v>
       </c>
@@ -5528,10 +5538,20 @@
       <c r="B24" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="52">
+      <c r="C24" s="58">
         <v>1899</v>
       </c>
-      <c r="D24" s="53"/>
+      <c r="D24" s="59"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="12"/>
       <c r="R24" s="16"/>
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
@@ -5541,70 +5561,70 @@
       <c r="B25" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="56">
+      <c r="C25" s="60">
         <v>1297</v>
       </c>
-      <c r="D25" s="57"/>
+      <c r="D25" s="61"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="58">
+      <c r="C26" s="62">
         <f>'Financial Model'!T47</f>
         <v>2341.395</v>
       </c>
-      <c r="D26" s="59"/>
+      <c r="D26" s="63"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B27" s="19"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="53"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="59"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B28" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="52" t="s">
+      <c r="C28" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="53"/>
+      <c r="D28" s="59"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="61"/>
+      <c r="D29" s="65"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="51"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="54">
+      <c r="C33" s="56">
         <f>C12/'Financial Model'!AA22</f>
         <v>11.245159106006854</v>
       </c>
-      <c r="D33" s="55"/>
+      <c r="D33" s="57"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="54">
+      <c r="C34" s="56">
         <f>C6/'Financial Model'!AA23</f>
         <v>7.8345184263332488</v>
       </c>
-      <c r="D34" s="55"/>
+      <c r="D34" s="57"/>
       <c r="H34" s="1" t="s">
         <v>11</v>
       </c>
@@ -5613,8 +5633,8 @@
       <c r="B35" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="52"/>
-      <c r="D35" s="53"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
       <c r="H35" s="1" t="s">
         <v>119</v>
       </c>
@@ -5623,49 +5643,41 @@
       <c r="B36" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="54">
+      <c r="C36" s="56">
         <f>C6/'Financial Model'!T73</f>
         <v>3.2184269795641627</v>
       </c>
-      <c r="D36" s="55"/>
+      <c r="D36" s="57"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="19"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="53"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="59"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="52"/>
-      <c r="D38" s="53"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="59"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="53"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="59"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="63"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="G5:P5"/>
     <mergeCell ref="R4:U4"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C23:D23"/>
@@ -5678,14 +5690,22 @@
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="H4:P4"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{12A2B318-E58C-4145-8299-C01CCCEE70D1}"/>
-    <hyperlink ref="P7" r:id="rId2" xr:uid="{459BEFFC-40F1-49A2-A3EA-13D4F85DB14A}"/>
+    <hyperlink ref="P8" r:id="rId2" xr:uid="{459BEFFC-40F1-49A2-A3EA-13D4F85DB14A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
@@ -5696,11 +5716,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9326757-89A0-4DD3-86DD-75EFD4F61FA8}">
   <dimension ref="B1:AN90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD15" sqref="AD15"/>
+      <selection pane="bottomRight" activeCell="V64" sqref="V64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7284,7 +7304,7 @@
         <v>528.029</v>
       </c>
       <c r="Z79" s="35">
-        <f t="shared" ref="Z79:AA79" si="16">Z45</f>
+        <f t="shared" ref="Z79" si="16">Z45</f>
         <v>815.75</v>
       </c>
       <c r="AA79" s="35">
@@ -7305,7 +7325,7 @@
         <v>5295.7790000000005</v>
       </c>
       <c r="Z80" s="35">
-        <f t="shared" ref="Z80:AA80" si="19">Z58+Z64</f>
+        <f t="shared" ref="Z80" si="19">Z58+Z64</f>
         <v>5720.21</v>
       </c>
       <c r="AA80" s="35">
@@ -7355,19 +7375,19 @@
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P84" s="64">
+      <c r="P84" s="49">
         <f t="shared" ref="P84" si="20">P83*P24</f>
         <v>31593.766230000001</v>
       </c>
-      <c r="T84" s="64">
+      <c r="T84" s="49">
         <f t="shared" ref="T84" si="21">T83*T24</f>
         <v>17153.538379999998</v>
       </c>
-      <c r="Z84" s="64">
+      <c r="Z84" s="49">
         <f t="shared" ref="Z84" si="22">Z83*Z24</f>
         <v>29590.400699999998</v>
       </c>
-      <c r="AA84" s="64">
+      <c r="AA84" s="49">
         <f>AA83*AA24</f>
         <v>22102.179329999999</v>
       </c>
@@ -7376,19 +7396,19 @@
       <c r="B85" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P85" s="64">
+      <c r="P85" s="49">
         <f>P84-P81</f>
         <v>35053.165229999999</v>
       </c>
-      <c r="T85" s="64">
+      <c r="T85" s="49">
         <f>T84-T81</f>
         <v>21921.288379999998</v>
       </c>
-      <c r="Z85" s="64">
+      <c r="Z85" s="49">
         <f>Z84-Z81</f>
         <v>34494.860699999997</v>
       </c>
-      <c r="AA85" s="64">
+      <c r="AA85" s="49">
         <f>AA84-AA81</f>
         <v>25745.959329999998</v>
       </c>
@@ -7397,19 +7417,19 @@
       <c r="B87" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P87" s="65">
+      <c r="P87" s="50">
         <f t="shared" ref="P87" si="23">P83/P73</f>
         <v>9.6498096321658622</v>
       </c>
-      <c r="T87" s="65">
+      <c r="T87" s="50">
         <f t="shared" ref="T87" si="24">T83/T73</f>
         <v>5.1166515127697503</v>
       </c>
-      <c r="Z87" s="65">
-        <f t="shared" ref="Z87:AA87" si="25">Z83/Z73</f>
+      <c r="Z87" s="50">
+        <f t="shared" ref="Z87" si="25">Z83/Z73</f>
         <v>9.6822886866655491</v>
       </c>
-      <c r="AA87" s="65">
+      <c r="AA87" s="50">
         <f>AA83/AA73</f>
         <v>6.2606234087970929</v>
       </c>
@@ -7418,12 +7438,12 @@
       <c r="B88" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="T88" s="65"/>
-      <c r="Z88" s="65">
-        <f t="shared" ref="Z88:AA88" si="26">Z84/Z8</f>
+      <c r="T88" s="50"/>
+      <c r="Z88" s="50">
+        <f t="shared" ref="Z88" si="26">Z84/Z8</f>
         <v>3.2028402714638258</v>
       </c>
-      <c r="AA88" s="65">
+      <c r="AA88" s="50">
         <f>AA84/AA8</f>
         <v>1.8664543675792531</v>
       </c>
@@ -7432,12 +7452,12 @@
       <c r="B89" s="1" t="s">
         <v>1373</v>
       </c>
-      <c r="T89" s="65"/>
-      <c r="Z89" s="65">
-        <f t="shared" ref="Z89:AA89" si="27">Z85/Z8</f>
+      <c r="T89" s="50"/>
+      <c r="Z89" s="50">
+        <f t="shared" ref="Z89" si="27">Z85/Z8</f>
         <v>3.7336949279127154</v>
       </c>
-      <c r="AA89" s="65">
+      <c r="AA89" s="50">
         <f>AA85/AA8</f>
         <v>2.1741592773058152</v>
       </c>
@@ -7446,12 +7466,12 @@
       <c r="B90" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="T90" s="65"/>
-      <c r="Z90" s="65">
-        <f t="shared" ref="Z90:AA90" si="28">Z83/Z23</f>
+      <c r="T90" s="50"/>
+      <c r="Z90" s="50">
+        <f t="shared" ref="Z90" si="28">Z83/Z23</f>
         <v>72.552343391794267</v>
       </c>
-      <c r="AA90" s="65">
+      <c r="AA90" s="50">
         <f>AA83/AA23</f>
         <v>15.936378537473129</v>
       </c>
@@ -7475,8 +7495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97EFD61D-7185-4A2D-B77C-954C6F6673F6}">
   <dimension ref="A1:G1212"/>
   <sheetViews>
-    <sheetView topLeftCell="A863" workbookViewId="0">
-      <selection activeCell="A883" sqref="A883:G883"/>
+    <sheetView topLeftCell="A1168" workbookViewId="0">
+      <selection activeCell="K1178" sqref="K1178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Start input Q3 results
</commit_message>
<xml_diff>
--- a/$VFC.xlsx
+++ b/$VFC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BB5435-CB30-4A98-94D0-D8E6EC9C04D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B59D5C-BA64-4727-AEDA-D523109C4EA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CCA103E1-675A-4605-B96F-0654FEFE97EB}"/>
   </bookViews>
@@ -4459,22 +4459,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4493,6 +4487,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4984,7 +4984,7 @@
   <dimension ref="A2:Z40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:P24"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5354,10 +5354,10 @@
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="59"/>
+      <c r="D16" s="55"/>
       <c r="G16" s="19"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -5382,10 +5382,10 @@
       <c r="B17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="59"/>
+      <c r="D17" s="55"/>
       <c r="G17" s="19"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -5431,10 +5431,10 @@
       <c r="B19" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="55"/>
+      <c r="D19" s="65"/>
       <c r="G19" s="19"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -5513,10 +5513,10 @@
       <c r="B23" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="58" t="s">
+      <c r="C23" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="59"/>
+      <c r="D23" s="55"/>
       <c r="G23" s="19"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -5538,10 +5538,10 @@
       <c r="B24" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="58">
+      <c r="C24" s="54">
         <v>1899</v>
       </c>
-      <c r="D24" s="59"/>
+      <c r="D24" s="55"/>
       <c r="G24" s="20"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -5561,43 +5561,43 @@
       <c r="B25" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="60">
+      <c r="C25" s="58">
         <v>1297</v>
       </c>
-      <c r="D25" s="61"/>
+      <c r="D25" s="59"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="62">
+      <c r="C26" s="60">
         <f>'Financial Model'!T47</f>
         <v>2341.395</v>
       </c>
-      <c r="D26" s="63"/>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B27" s="19"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="59"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B28" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="59"/>
+      <c r="D28" s="55"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="65"/>
+      <c r="D29" s="63"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B32" s="51" t="s">
@@ -5633,8 +5633,8 @@
       <c r="B35" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="55"/>
       <c r="H35" s="1" t="s">
         <v>119</v>
       </c>
@@ -5651,37 +5651,39 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="19"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="59"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="55"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="59"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="55"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="59"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="G5:P5"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
@@ -5690,18 +5692,16 @@
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="B32:D32"/>
+    <mergeCell ref="G5:P5"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="W4:Z4"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{12A2B318-E58C-4145-8299-C01CCCEE70D1}"/>
@@ -5720,7 +5720,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V64" sqref="V64"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5782,7 +5782,7 @@
       <c r="T1" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="32" t="s">
         <v>150</v>
       </c>
       <c r="W1" s="21" t="s">
@@ -5855,6 +5855,9 @@
       <c r="T2" s="33">
         <v>44744</v>
       </c>
+      <c r="U2" s="33">
+        <v>44834</v>
+      </c>
       <c r="Y2" s="33">
         <v>43918</v>
       </c>
@@ -5881,6 +5884,9 @@
       <c r="T3" s="34">
         <v>946.8</v>
       </c>
+      <c r="U3" s="34">
+        <v>952.1</v>
+      </c>
       <c r="Y3" s="35">
         <v>4063.4</v>
       </c>
@@ -5907,6 +5913,9 @@
       <c r="T4" s="34">
         <v>481.1</v>
       </c>
+      <c r="U4" s="34">
+        <v>950.8</v>
+      </c>
       <c r="Y4" s="35">
         <v>2699.8</v>
       </c>
@@ -5933,6 +5942,9 @@
       <c r="T5" s="34">
         <v>269.5</v>
       </c>
+      <c r="U5" s="34">
+        <v>524.20000000000005</v>
+      </c>
       <c r="Y5" s="35">
         <v>1768.8</v>
       </c>
@@ -5959,6 +5971,9 @@
       <c r="T6" s="34">
         <v>170.4</v>
       </c>
+      <c r="U6" s="34">
+        <v>186.4</v>
+      </c>
       <c r="Y6" s="35">
         <v>645.1</v>
       </c>
@@ -5985,6 +6000,9 @@
       <c r="T7" s="34">
         <v>393.9</v>
       </c>
+      <c r="U7" s="34">
+        <v>467.1</v>
+      </c>
       <c r="Y7" s="35">
         <f>Y8-SUM(Y3:Y6)</f>
         <v>1311.4560000000001</v>
@@ -6016,7 +6034,10 @@
         <f>SUM(T3:T7)</f>
         <v>2261.7000000000003</v>
       </c>
-      <c r="U8" s="36"/>
+      <c r="U8" s="36">
+        <f>SUM(U3:U7)</f>
+        <v>3080.6000000000004</v>
+      </c>
       <c r="Y8" s="36">
         <v>10488.556</v>
       </c>
@@ -6039,6 +6060,9 @@
       <c r="S9" s="42"/>
       <c r="T9" s="42">
         <v>1042.982</v>
+      </c>
+      <c r="U9" s="42">
+        <v>1498.1769999999999</v>
       </c>
       <c r="Y9" s="42">
         <v>4690.5200000000004</v>
@@ -6063,6 +6087,10 @@
         <f>T8-T9</f>
         <v>1218.7180000000003</v>
       </c>
+      <c r="U10" s="36">
+        <f>U8-U9</f>
+        <v>1582.4230000000005</v>
+      </c>
       <c r="Y10" s="36">
         <f>Y8-Y9</f>
         <v>5798.0360000000001</v>
@@ -6086,6 +6114,9 @@
       <c r="T11" s="42">
         <v>1155.251</v>
       </c>
+      <c r="U11" s="42">
+        <v>1251.32</v>
+      </c>
       <c r="Y11" s="42">
         <v>4547.0079999999998</v>
       </c>
@@ -6106,6 +6137,9 @@
       <c r="T12" s="1">
         <v>0</v>
       </c>
+      <c r="U12" s="42">
+        <v>421.92200000000003</v>
+      </c>
       <c r="Y12" s="42">
         <v>323.22300000000001</v>
       </c>
@@ -6128,6 +6162,10 @@
         <f>T10-T11-T12</f>
         <v>63.467000000000326</v>
       </c>
+      <c r="U13" s="36">
+        <f>U10-U11-U12</f>
+        <v>-90.818999999999505</v>
+      </c>
       <c r="Y13" s="36">
         <f>Y10-Y11-Y12</f>
         <v>927.80500000000029</v>
@@ -6151,6 +6189,9 @@
       <c r="T14" s="1">
         <v>0</v>
       </c>
+      <c r="U14" s="42">
+        <v>0</v>
+      </c>
       <c r="Y14" s="42">
         <v>19.867000000000001</v>
       </c>
@@ -6171,6 +6212,9 @@
       <c r="T15" s="1">
         <v>31.262</v>
       </c>
+      <c r="U15" s="42">
+        <v>33.902999999999999</v>
+      </c>
       <c r="Y15" s="42">
         <v>92.042000000000002</v>
       </c>
@@ -6191,6 +6235,9 @@
       <c r="T16" s="1">
         <v>0</v>
       </c>
+      <c r="U16" s="42">
+        <v>0</v>
+      </c>
       <c r="Y16" s="42">
         <v>59.771999999999998</v>
       </c>
@@ -6211,6 +6258,9 @@
       <c r="T17" s="1">
         <v>-94.713999999999999</v>
       </c>
+      <c r="U17" s="42">
+        <v>-9.2799999999999994</v>
+      </c>
       <c r="Y17" s="42">
         <v>-68.650000000000006</v>
       </c>
@@ -6233,6 +6283,10 @@
         <f>T13+T14-T15-T16+T17</f>
         <v>-62.508999999999673</v>
       </c>
+      <c r="U18" s="42">
+        <f>U13+U14-U15-U16+U17</f>
+        <v>-134.0019999999995</v>
+      </c>
       <c r="Y18" s="42">
         <f>Y13+Y14-Y15-Y16+Y17</f>
         <v>727.2080000000002</v>
@@ -6256,6 +6310,9 @@
       <c r="T19" s="1">
         <v>-6.6539999999999999</v>
       </c>
+      <c r="U19" s="42">
+        <v>-15.57</v>
+      </c>
       <c r="Y19" s="42">
         <v>98.061999999999998</v>
       </c>
@@ -6277,6 +6334,10 @@
         <f>T18-T19</f>
         <v>-55.854999999999677</v>
       </c>
+      <c r="U20" s="42">
+        <f>U18-U19</f>
+        <v>-118.4319999999995</v>
+      </c>
       <c r="Y20" s="42">
         <f>Y18-Y19</f>
         <v>629.14600000000019</v>
@@ -6300,6 +6361,9 @@
       <c r="T21" s="1">
         <v>0</v>
       </c>
+      <c r="U21" s="42">
+        <v>0</v>
+      </c>
       <c r="Y21" s="42">
         <v>50.302999999999997</v>
       </c>
@@ -6322,6 +6386,10 @@
         <f>T20+T21</f>
         <v>-55.854999999999677</v>
       </c>
+      <c r="U22" s="36">
+        <f>U20+U21</f>
+        <v>-118.4319999999995</v>
+      </c>
       <c r="Y22" s="36">
         <f>Y20+Y21</f>
         <v>679.44900000000018</v>
@@ -6347,6 +6415,10 @@
         <f>T22/T24</f>
         <v>-0.14411850460441186</v>
       </c>
+      <c r="U23" s="47">
+        <f>U22/U24</f>
+        <v>-0.30548275933224528</v>
+      </c>
       <c r="Y23" s="42">
         <f>Y22/Y24</f>
         <v>1.7183361110338362</v>
@@ -6369,6 +6441,9 @@
       </c>
       <c r="T24" s="42">
         <v>387.56299999999999</v>
+      </c>
+      <c r="U24" s="46">
+        <v>387.68799999999999</v>
       </c>
       <c r="Y24" s="42">
         <v>395.411</v>
@@ -6607,18 +6682,21 @@
       <c r="M31" s="41"/>
       <c r="N31" s="41"/>
       <c r="O31" s="41"/>
-      <c r="P31" s="41"/>
+      <c r="P31" s="41">
+        <f>P8/O8-1</f>
+        <v>-0.15026909823053403</v>
+      </c>
       <c r="Q31" s="41"/>
       <c r="R31" s="41"/>
-      <c r="S31" s="41">
-        <f t="shared" ref="S31:T31" si="2">S7/O7-1</f>
-        <v>0.11394689352926024</v>
-      </c>
+      <c r="S31" s="41"/>
       <c r="T31" s="41">
-        <f t="shared" si="2"/>
-        <v>9.4774874930516839E-2</v>
-      </c>
-      <c r="U31" s="41"/>
+        <f>T8/S8-1</f>
+        <v>-0.19931320140191866</v>
+      </c>
+      <c r="U31" s="41">
+        <f>U8/T8-1</f>
+        <v>0.36207277711455976</v>
+      </c>
       <c r="V31" s="41"/>
       <c r="W31" s="41"/>
       <c r="X31" s="41"/>
@@ -6660,11 +6738,15 @@
         <v>0.85170372733072086</v>
       </c>
       <c r="T35" s="39">
-        <f t="shared" ref="T35" si="3">T10/T8</f>
+        <f t="shared" ref="T35:U35" si="2">T10/T8</f>
         <v>0.53885042224875102</v>
       </c>
+      <c r="U35" s="39">
+        <f t="shared" si="2"/>
+        <v>0.51367363500616769</v>
+      </c>
       <c r="Y35" s="39">
-        <f t="shared" ref="Y35" si="4">Y10/Y8</f>
+        <f t="shared" ref="Y35" si="3">Y10/Y8</f>
         <v>0.55279640019083653</v>
       </c>
       <c r="Z35" s="39">
@@ -6681,19 +6763,23 @@
         <v>111</v>
       </c>
       <c r="P36" s="39">
-        <f t="shared" ref="P36" si="5">P13/P8</f>
+        <f t="shared" ref="P36" si="4">P13/P8</f>
         <v>0.37958033354597642</v>
       </c>
       <c r="T36" s="39">
-        <f t="shared" ref="T36" si="6">T13/T8</f>
+        <f t="shared" ref="T36:U36" si="5">T13/T8</f>
         <v>2.8061635053278647E-2</v>
       </c>
+      <c r="U36" s="39">
+        <f t="shared" si="5"/>
+        <v>-2.9480945270401706E-2</v>
+      </c>
       <c r="Y36" s="39">
-        <f t="shared" ref="Y36:Z36" si="7">Y13/Y8</f>
+        <f t="shared" ref="Y36:Z36" si="6">Y13/Y8</f>
         <v>8.8458792611680798E-2</v>
       </c>
       <c r="Z36" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>6.5766225050872554E-2</v>
       </c>
       <c r="AA36" s="39">
@@ -6706,19 +6792,23 @@
         <v>112</v>
       </c>
       <c r="P37" s="39">
-        <f t="shared" ref="P37" si="8">P22/P8</f>
+        <f t="shared" ref="P37" si="7">P22/P8</f>
         <v>0.14774674200309854</v>
       </c>
       <c r="T37" s="39">
-        <f t="shared" ref="T37" si="9">T22/T8</f>
+        <f t="shared" ref="T37:U37" si="8">T22/T8</f>
         <v>-2.4696025113852268E-2</v>
       </c>
+      <c r="U37" s="39">
+        <f t="shared" si="8"/>
+        <v>-3.8444458871648213E-2</v>
+      </c>
       <c r="Y37" s="39">
-        <f t="shared" ref="Y37:Z37" si="10">Y22/Y8</f>
+        <f t="shared" ref="Y37:Z37" si="9">Y22/Y8</f>
         <v>6.4780032637476517E-2</v>
       </c>
       <c r="Z37" s="39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>4.4145235311945419E-2</v>
       </c>
       <c r="AA37" s="39">
@@ -6731,19 +6821,23 @@
         <v>113</v>
       </c>
       <c r="P38" s="39">
-        <f t="shared" ref="P38" si="11">P19/P18</f>
+        <f t="shared" ref="P38" si="10">P19/P18</f>
         <v>3.1111105619349239E-2</v>
       </c>
       <c r="T38" s="39">
-        <f t="shared" ref="T38" si="12">T19/T18</f>
+        <f t="shared" ref="T38:U38" si="11">T19/T18</f>
         <v>0.10644867139132021</v>
       </c>
+      <c r="U38" s="39">
+        <f t="shared" si="11"/>
+        <v>0.11619229563737898</v>
+      </c>
       <c r="Y38" s="39">
-        <f t="shared" ref="Y38:Z38" si="13">Y19/Y18</f>
+        <f t="shared" ref="Y38:Z38" si="12">Y19/Y18</f>
         <v>0.13484725140537504</v>
       </c>
       <c r="Z38" s="39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0.22249486243597147</v>
       </c>
       <c r="AA38" s="39">
@@ -7296,15 +7390,15 @@
         <v>6</v>
       </c>
       <c r="P79" s="35">
-        <f t="shared" ref="P79" si="14">P45</f>
+        <f t="shared" ref="P79" si="13">P45</f>
         <v>1274.9259999999999</v>
       </c>
       <c r="T79" s="35">
-        <f t="shared" ref="T79" si="15">T45</f>
+        <f t="shared" ref="T79" si="14">T45</f>
         <v>528.029</v>
       </c>
       <c r="Z79" s="35">
-        <f t="shared" ref="Z79" si="16">Z45</f>
+        <f t="shared" ref="Z79" si="15">Z45</f>
         <v>815.75</v>
       </c>
       <c r="AA79" s="35">
@@ -7317,15 +7411,15 @@
         <v>7</v>
       </c>
       <c r="P80" s="35">
-        <f t="shared" ref="P80" si="17">P58+P64</f>
+        <f t="shared" ref="P80" si="16">P58+P64</f>
         <v>4734.3250000000007</v>
       </c>
       <c r="T80" s="35">
-        <f t="shared" ref="T80" si="18">T58+T64</f>
+        <f t="shared" ref="T80" si="17">T58+T64</f>
         <v>5295.7790000000005</v>
       </c>
       <c r="Z80" s="35">
-        <f t="shared" ref="Z80" si="19">Z58+Z64</f>
+        <f t="shared" ref="Z80" si="18">Z58+Z64</f>
         <v>5720.21</v>
       </c>
       <c r="AA80" s="35">
@@ -7376,15 +7470,15 @@
         <v>5</v>
       </c>
       <c r="P84" s="49">
-        <f t="shared" ref="P84" si="20">P83*P24</f>
+        <f t="shared" ref="P84" si="19">P83*P24</f>
         <v>31593.766230000001</v>
       </c>
       <c r="T84" s="49">
-        <f t="shared" ref="T84" si="21">T83*T24</f>
+        <f t="shared" ref="T84" si="20">T83*T24</f>
         <v>17153.538379999998</v>
       </c>
       <c r="Z84" s="49">
-        <f t="shared" ref="Z84" si="22">Z83*Z24</f>
+        <f t="shared" ref="Z84" si="21">Z83*Z24</f>
         <v>29590.400699999998</v>
       </c>
       <c r="AA84" s="49">
@@ -7418,15 +7512,15 @@
         <v>85</v>
       </c>
       <c r="P87" s="50">
-        <f t="shared" ref="P87" si="23">P83/P73</f>
+        <f t="shared" ref="P87" si="22">P83/P73</f>
         <v>9.6498096321658622</v>
       </c>
       <c r="T87" s="50">
-        <f t="shared" ref="T87" si="24">T83/T73</f>
+        <f t="shared" ref="T87" si="23">T83/T73</f>
         <v>5.1166515127697503</v>
       </c>
       <c r="Z87" s="50">
-        <f t="shared" ref="Z87" si="25">Z83/Z73</f>
+        <f t="shared" ref="Z87" si="24">Z83/Z73</f>
         <v>9.6822886866655491</v>
       </c>
       <c r="AA87" s="50">
@@ -7440,7 +7534,7 @@
       </c>
       <c r="T88" s="50"/>
       <c r="Z88" s="50">
-        <f t="shared" ref="Z88" si="26">Z84/Z8</f>
+        <f t="shared" ref="Z88" si="25">Z84/Z8</f>
         <v>3.2028402714638258</v>
       </c>
       <c r="AA88" s="50">
@@ -7454,7 +7548,7 @@
       </c>
       <c r="T89" s="50"/>
       <c r="Z89" s="50">
-        <f t="shared" ref="Z89" si="27">Z85/Z8</f>
+        <f t="shared" ref="Z89" si="26">Z85/Z8</f>
         <v>3.7336949279127154</v>
       </c>
       <c r="AA89" s="50">
@@ -7468,7 +7562,7 @@
       </c>
       <c r="T90" s="50"/>
       <c r="Z90" s="50">
-        <f t="shared" ref="Z90" si="28">Z83/Z23</f>
+        <f t="shared" ref="Z90" si="27">Z83/Z23</f>
         <v>72.552343391794267</v>
       </c>
       <c r="AA90" s="50">
@@ -7481,13 +7575,14 @@
     <hyperlink ref="AA1" r:id="rId1" xr:uid="{E361DF71-81CD-44B3-92EA-C93A48C261DE}"/>
     <hyperlink ref="T1" r:id="rId2" xr:uid="{FD66D2D5-10E8-46D6-9236-49BEBA00F0EC}"/>
     <hyperlink ref="Y1" r:id="rId3" xr:uid="{62807AAA-DD69-44A4-AFA7-591172D41776}"/>
+    <hyperlink ref="U1" r:id="rId4" xr:uid="{9531B1A7-B365-4021-B8C5-6A1EC1D04E83}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
   <ignoredErrors>
-    <ignoredError sqref="O8:P8 S8:T8 Z8:AA8 Y7" formulaRange="1"/>
+    <ignoredError sqref="O8:P8 S8:U8 Z8:AA8 Y7" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>